<commit_message>
added additional folders in Abigail
</commit_message>
<xml_diff>
--- a/Planets/misc/Actual vs Simulation.xlsx
+++ b/Planets/misc/Actual vs Simulation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\VS Code\Abigail - vsCode\Planets\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D089F0F6-227A-4FED-84F7-A15CB02598C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AE171B-BEB5-422D-BF14-1BB7F36DF3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4BE2928A-1D5D-4009-AE43-83C9699A86DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4BE2928A-1D5D-4009-AE43-83C9699A86DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>Mercury</t>
   </si>
@@ -174,6 +174,15 @@
   </si>
   <si>
     <t>ACT</t>
+  </si>
+  <si>
+    <t>MARS: average -0.88% is closer to the sun</t>
+  </si>
+  <si>
+    <t>MARS: minimum 8.38% is further from the sun</t>
+  </si>
+  <si>
+    <t>MARS: maximum -9.15% is closer to the sun</t>
   </si>
 </sst>
 </file>
@@ -446,7 +455,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -499,6 +508,30 @@
     <xf numFmtId="10" fontId="3" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -514,29 +547,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -854,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87ECA6CB-7DE9-4962-BB31-2ECBD6500398}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -872,443 +884,506 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="28.5" x14ac:dyDescent="0.3">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-    </row>
-    <row r="4" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:14" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="18" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+    </row>
+    <row r="2" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:14" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C3" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="20" t="s">
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="21"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="20" t="s">
+      <c r="G3" s="29"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="21"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="20" t="s">
+      <c r="J3" s="29"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="21"/>
-      <c r="N5" s="22"/>
-    </row>
-    <row r="6" spans="1:14" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="19"/>
-      <c r="C6" s="6" t="s">
+      <c r="M3" s="29"/>
+      <c r="N3" s="30"/>
+    </row>
+    <row r="4" spans="1:14" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="27"/>
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="6" t="s">
+      <c r="L4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="M4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N4" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="21.75" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="5" t="s">
+    <row r="5" spans="1:14" ht="21.75" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C5" s="9">
         <v>56.9</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D5" s="10">
         <v>57.9</v>
       </c>
-      <c r="E7" s="11">
-        <f>(C7-D7)/C7</f>
+      <c r="E5" s="11">
+        <f>(C5-D5)/C5</f>
         <v>-1.7574692442882251E-2</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F5" s="9">
         <v>108.1</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G5" s="10">
         <v>108.2</v>
       </c>
-      <c r="H7" s="11">
-        <f>(F7-G7)/F7</f>
+      <c r="H5" s="11">
+        <f>(F5-G5)/F5</f>
         <v>-9.2506938020359424E-4</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I5" s="9">
         <v>149.4</v>
       </c>
-      <c r="J7" s="10">
+      <c r="J5" s="10">
         <v>149.6</v>
       </c>
-      <c r="K7" s="11">
-        <f>(I7-J7)/I7</f>
+      <c r="K5" s="11">
+        <f>(I5-J5)/I5</f>
         <v>-1.3386880856759613E-3</v>
       </c>
-      <c r="L7" s="9">
+      <c r="L5" s="9">
         <v>226</v>
       </c>
-      <c r="M7" s="10">
+      <c r="M5" s="10">
         <v>228</v>
       </c>
-      <c r="N7" s="11">
-        <f>(L7-M7)/L7</f>
+      <c r="N5" s="11">
+        <f>(L5-M5)/L5</f>
         <v>-8.8495575221238937E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="21" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+    <row r="6" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C6" s="12">
         <v>54.6</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D6" s="13">
         <v>46</v>
       </c>
-      <c r="E8" s="14">
-        <f t="shared" ref="E8:E9" si="0">(C8-D8)/C8</f>
+      <c r="E6" s="14">
+        <f t="shared" ref="E6:E7" si="0">(C6-D6)/C6</f>
         <v>0.15750915750915753</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F6" s="12">
         <v>106.6</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G6" s="13">
         <v>107.5</v>
       </c>
-      <c r="H8" s="14">
-        <f t="shared" ref="H8:H9" si="1">(F8-G8)/F8</f>
+      <c r="H6" s="14">
+        <f t="shared" ref="H6:H7" si="1">(F6-G6)/F6</f>
         <v>-8.4427767354597165E-3</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I6" s="12">
         <v>148.30000000000001</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J6" s="13">
         <v>147.1</v>
       </c>
-      <c r="K8" s="14">
-        <f t="shared" ref="K8:K9" si="2">(I8-J8)/I8</f>
+      <c r="K6" s="14">
+        <f t="shared" ref="K6:K7" si="2">(I6-J6)/I6</f>
         <v>8.0917060013487325E-3</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L6" s="12">
         <v>225.6</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M6" s="13">
         <v>206.7</v>
       </c>
-      <c r="N8" s="14">
-        <f t="shared" ref="N8:N9" si="3">(L8-M8)/L8</f>
+      <c r="N6" s="14">
+        <f t="shared" ref="N6:N7" si="3">(L6-M6)/L6</f>
         <v>8.3776595744680882E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="4" t="s">
+    <row r="7" spans="1:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C7" s="15">
         <v>59.1</v>
       </c>
-      <c r="D9" s="16">
+      <c r="D7" s="16">
         <v>69.8</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E7" s="17">
         <f t="shared" si="0"/>
         <v>-0.18104906937394238</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F7" s="15">
         <v>109.6</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G7" s="16">
         <v>108.9</v>
       </c>
-      <c r="H9" s="17">
+      <c r="H7" s="17">
         <f t="shared" si="1"/>
         <v>6.3868613138685099E-3</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I7" s="15">
         <v>150.9</v>
       </c>
-      <c r="J9" s="16">
+      <c r="J7" s="16">
         <v>152.1</v>
       </c>
-      <c r="K9" s="17">
+      <c r="K7" s="17">
         <f t="shared" si="2"/>
         <v>-7.9522862823060876E-3</v>
       </c>
-      <c r="L9" s="15">
+      <c r="L7" s="15">
         <v>228.4</v>
       </c>
-      <c r="M9" s="16">
+      <c r="M7" s="16">
         <v>249.3</v>
       </c>
-      <c r="N9" s="17">
+      <c r="N7" s="17">
         <f t="shared" si="3"/>
         <v>-9.1506129597197922E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="19.5" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="1" t="s">
+    <row r="8" spans="1:14" ht="19.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="24">
-        <f>AVERAGE(C8:C9)</f>
+      <c r="C9" s="18">
+        <f>AVERAGE(C6:C7)</f>
         <v>56.85</v>
       </c>
-      <c r="D11" s="24">
-        <f t="shared" ref="D11:N11" si="4">AVERAGE(D8:D9)</f>
+      <c r="D9" s="18">
+        <f t="shared" ref="D9:M9" si="4">AVERAGE(D6:D7)</f>
         <v>57.9</v>
       </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24">
+      <c r="E9" s="18"/>
+      <c r="F9" s="18">
         <f t="shared" si="4"/>
         <v>108.1</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G9" s="18">
         <f t="shared" si="4"/>
         <v>108.2</v>
       </c>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24">
+      <c r="H9" s="18"/>
+      <c r="I9" s="18">
         <f t="shared" si="4"/>
         <v>149.60000000000002</v>
       </c>
-      <c r="J11" s="24">
+      <c r="J9" s="18">
         <f t="shared" si="4"/>
         <v>149.6</v>
       </c>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24">
+      <c r="K9" s="18"/>
+      <c r="L9" s="18">
         <f t="shared" si="4"/>
         <v>227</v>
       </c>
-      <c r="M11" s="24">
+      <c r="M9" s="18">
         <f t="shared" si="4"/>
         <v>228</v>
       </c>
-      <c r="N11" s="24"/>
+      <c r="N9" s="18"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="23">
+        <v>149.59787069999999</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="F11" s="19"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C12" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="30">
-        <v>149.59787069999999</v>
-      </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="F13" s="25"/>
+      <c r="C13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C14" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
+      <c r="B14" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2">
+        <f t="shared" ref="C14:D16" si="5">C5/$B$11</f>
+        <v>0.38035300725707455</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="5"/>
+        <v>0.38703759437934304</v>
+      </c>
+      <c r="E14" s="31">
+        <f t="shared" ref="E14:E16" si="6">(C14-D14)/C14</f>
+        <v>-1.7574692442882373E-2</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" ref="F14:G16" si="7">F5/$B$11</f>
+        <v>0.72260386791721898</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="7"/>
+        <v>0.72327232662944585</v>
+      </c>
+      <c r="H14" s="31">
+        <f t="shared" ref="H14:H16" si="8">(F14-G14)/F14</f>
+        <v>-9.250693802035525E-4</v>
+      </c>
+      <c r="I14" s="2">
+        <f t="shared" ref="I14:J16" si="9">I5/$B$11</f>
+        <v>0.99867731606690591</v>
+      </c>
+      <c r="J14" s="2">
+        <f t="shared" si="9"/>
+        <v>1.0000142334913595</v>
+      </c>
+      <c r="K14" s="31">
+        <f t="shared" ref="K14:K16" si="10">(I14-J14)/I14</f>
+        <v>-1.33868808567598E-3</v>
+      </c>
+      <c r="L14" s="2">
+        <f t="shared" ref="L14:M16" si="11">L5/$B$11</f>
+        <v>1.5107166896326689</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="11"/>
+        <v>1.5240858638772057</v>
+      </c>
+      <c r="N14" s="31">
+        <f t="shared" ref="N14:N16" si="12">(L14-M14)/L14</f>
+        <v>-8.8495575221238087E-3</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>20</v>
+      <c r="B15" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="2">
+        <f t="shared" si="5"/>
+        <v>0.36497845687585717</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="5"/>
+        <v>0.3074910076243485</v>
+      </c>
+      <c r="E15" s="31">
+        <f t="shared" si="6"/>
+        <v>0.15750915750915759</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="7"/>
+        <v>0.71257698723381635</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="7"/>
+        <v>0.71859311564385797</v>
+      </c>
+      <c r="H15" s="31">
+        <f t="shared" si="8"/>
+        <v>-8.4427767354596905E-3</v>
+      </c>
+      <c r="I15" s="2">
+        <f t="shared" si="9"/>
+        <v>0.99132427023241065</v>
+      </c>
+      <c r="J15" s="2">
+        <f t="shared" si="9"/>
+        <v>0.98330276568568842</v>
+      </c>
+      <c r="K15" s="31">
+        <f t="shared" si="10"/>
+        <v>8.0917060013487186E-3</v>
+      </c>
+      <c r="L15" s="2">
+        <f t="shared" si="11"/>
+        <v>1.5080428547837614</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="11"/>
+        <v>1.3817041581728877</v>
+      </c>
+      <c r="N15" s="31">
+        <f t="shared" si="12"/>
+        <v>8.377659574468091E-2</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="25" t="s">
-        <v>15</v>
+      <c r="B16" s="19" t="s">
+        <v>17</v>
       </c>
       <c r="C16" s="2">
-        <f>C7/$B$13</f>
-        <v>0.38035300725707455</v>
+        <f t="shared" si="5"/>
+        <v>0.39505909892606517</v>
       </c>
       <c r="D16" s="2">
-        <f>D7/$B$13</f>
-        <v>0.38703759437934304</v>
+        <f t="shared" si="5"/>
+        <v>0.46658418113433753</v>
+      </c>
+      <c r="E16" s="31">
+        <f t="shared" si="6"/>
+        <v>-0.18104906937394244</v>
       </c>
       <c r="F16" s="2">
-        <f>F7/$B$13</f>
-        <v>0.72260386791721898</v>
+        <f t="shared" si="7"/>
+        <v>0.73263074860062161</v>
       </c>
       <c r="G16" s="2">
-        <f>G7/$B$13</f>
-        <v>0.72327232662944585</v>
+        <f t="shared" si="7"/>
+        <v>0.72795153761503384</v>
+      </c>
+      <c r="H16" s="31">
+        <f t="shared" si="8"/>
+        <v>6.3868613138684163E-3</v>
       </c>
       <c r="I16" s="2">
-        <f>I7/$B$13</f>
-        <v>0.99867731606690591</v>
+        <f t="shared" si="9"/>
+        <v>1.0087041967503085</v>
       </c>
       <c r="J16" s="2">
-        <f>J7/$B$13</f>
-        <v>1.0000142334913595</v>
+        <f t="shared" si="9"/>
+        <v>1.0167257012970305</v>
+      </c>
+      <c r="K16" s="31">
+        <f t="shared" si="10"/>
+        <v>-7.9522862823060425E-3</v>
       </c>
       <c r="L16" s="2">
-        <f>L7/$B$13</f>
-        <v>1.5107166896326689</v>
+        <f t="shared" si="11"/>
+        <v>1.5267596987261132</v>
       </c>
       <c r="M16" s="2">
-        <f>M7/$B$13</f>
-        <v>1.5240858638772057</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B17" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="2">
-        <f>C8/$B$13</f>
-        <v>0.36497845687585717</v>
-      </c>
-      <c r="D17" s="2">
-        <f>D8/$B$13</f>
-        <v>0.3074910076243485</v>
-      </c>
-      <c r="F17" s="2">
-        <f>F8/$B$13</f>
-        <v>0.71257698723381635</v>
-      </c>
-      <c r="G17" s="2">
-        <f>G8/$B$13</f>
-        <v>0.71859311564385797</v>
-      </c>
-      <c r="I17" s="2">
-        <f>I8/$B$13</f>
-        <v>0.99132427023241065</v>
-      </c>
-      <c r="J17" s="2">
-        <f>J8/$B$13</f>
-        <v>0.98330276568568842</v>
-      </c>
-      <c r="L17" s="2">
-        <f>L8/$B$13</f>
-        <v>1.5080428547837614</v>
-      </c>
-      <c r="M17" s="2">
-        <f>M8/$B$13</f>
-        <v>1.3817041581728877</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="2">
-        <f>C9/$B$13</f>
-        <v>0.39505909892606517</v>
-      </c>
-      <c r="D18" s="2">
-        <f>D9/$B$13</f>
-        <v>0.46658418113433753</v>
-      </c>
-      <c r="F18" s="2">
-        <f>F9/$B$13</f>
-        <v>0.73263074860062161</v>
-      </c>
-      <c r="G18" s="2">
-        <f>G9/$B$13</f>
-        <v>0.72795153761503384</v>
-      </c>
-      <c r="I18" s="2">
-        <f>I9/$B$13</f>
-        <v>1.0087041967503085</v>
-      </c>
-      <c r="J18" s="2">
-        <f>J9/$B$13</f>
-        <v>1.0167257012970305</v>
-      </c>
-      <c r="L18" s="2">
-        <f>L9/$B$13</f>
-        <v>1.5267596987261132</v>
-      </c>
-      <c r="M18" s="2">
-        <f>M9/$B$13</f>
+        <f t="shared" si="11"/>
         <v>1.6664675695815236</v>
       </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="D20" s="28" t="s">
+      <c r="N16" s="31">
+        <f t="shared" si="12"/>
+        <v>-9.1506129597197866E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D18" s="21" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="I19" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="I20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="I21" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="B1:N1"/>
-    <mergeCell ref="C14:L14"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="C12:L12"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="L3:N3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D20" r:id="rId1" xr:uid="{235F7498-3849-4152-97AB-4794894D1AB2}"/>
+    <hyperlink ref="D18" r:id="rId1" xr:uid="{235F7498-3849-4152-97AB-4794894D1AB2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>

</xml_diff>

<commit_message>
created new branch  063023-08-09AM
</commit_message>
<xml_diff>
--- a/Planets/misc/Actual vs Simulation.xlsx
+++ b/Planets/misc/Actual vs Simulation.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\VS Code\Abigail - vsCode\Planets\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E230FB-244D-4DFD-A96B-FBF9644D95C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABB07C4-E4CB-4BA4-95AE-16823B5119D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4BE2928A-1D5D-4009-AE43-83C9699A86DE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Orig" sheetId="1" r:id="rId1"/>
+    <sheet name="Copy" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="31">
   <si>
     <t>Venus</t>
   </si>
@@ -157,62 +158,6 @@
     <t xml:space="preserve">Mercury </t>
   </si>
   <si>
-    <r>
-      <t>(10</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>6</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> km)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Maximum DTS - 10</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>6</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> km</t>
-    </r>
-  </si>
-  <si>
     <t>bad input</t>
   </si>
   <si>
@@ -224,6 +169,151 @@
   <si>
     <t>numerical method (Euler's Method)</t>
   </si>
+  <si>
+    <r>
+      <t>(10</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> km)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Minimum DTS </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (10</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> km)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Average DTS  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(10</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> km)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Maximum DTS  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(10</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>6</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> km)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -233,7 +323,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000000000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -306,6 +396,29 @@
     <font>
       <sz val="16"/>
       <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -570,12 +683,6 @@
     <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -585,37 +692,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="9" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="10" fontId="9" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="9" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -633,11 +713,44 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -700,7 +813,7 @@
             </a:br>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="1"/>
-              <a:t>(Distance from the Sun - 10</a:t>
+              <a:t>(Distance To The Sun - 10</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1200" b="1" baseline="30000"/>
@@ -802,7 +915,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Perihelion</c:v>
+            <c:v>Perihelion (min)</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -825,7 +938,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$D$5</c:f>
+              <c:f>Orig!$C$5:$D$5</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
@@ -838,6 +951,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:shape val="pyramidToMax"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5E8B-4D9B-B655-6B5DE5BE9932}"/>
@@ -871,7 +985,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$D$6</c:f>
+              <c:f>Orig!$C$6:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
@@ -884,6 +998,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:shape val="pyramidToMax"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5E8B-4D9B-B655-6B5DE5BE9932}"/>
@@ -894,7 +1009,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Aphelion</c:v>
+            <c:v>Aphelion (max)</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -917,7 +1032,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$D$7</c:f>
+              <c:f>Orig!$C$7:$D$7</c:f>
               <c:numCache>
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
@@ -930,6 +1045,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:shape val="pyramidToMax"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-5E8B-4D9B-B655-6B5DE5BE9932}"/>
@@ -958,6 +1074,651 @@
         <c:delete val="1"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Nasa Actual</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>   vs   Simulation</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="267319743"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="267319743"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance from the Sum (10</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="30000"/>
+                  <a:t>6</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t> km)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="5.7507144256754815E-3"/>
+              <c:y val="0.40793053532599699"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="267324063"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:serAx>
+        <c:axId val="463152175"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="267319743"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="1"/>
+              <a:t>MERCURY</a:t>
+            </a:r>
+            <a:br>
+              <a:rPr lang="en-US" sz="1200" b="1"/>
+            </a:br>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="1"/>
+              <a:t>(Distance To The Sun - 10</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="1" baseline="30000"/>
+              <a:t>6</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1200" b="1"/>
+              <a:t> km)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.7489142475339796E-2"/>
+          <c:y val="0.14856481481481484"/>
+          <c:w val="0.78230035856527569"/>
+          <c:h val="0.72088764946048411"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:bar3DChart>
+        <c:barDir val="col"/>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Perihelion (min)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Simulation              Actual</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Copy!$C$5:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>54.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="pyramidToMax"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BA1C-48C0-87DF-BA03AE87A974}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Average</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Simulation              Actual</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Copy!$C$6:$D$6</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>56.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>57.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="pyramidToMax"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BA1C-48C0-87DF-BA03AE87A974}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Aphelion (max)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+            <a:sp3d/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="1"/>
+              <c:pt idx="0">
+                <c:v>Simulation              Actual</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Copy!$C$7:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>59.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>69.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="pyramidToMax"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BA1C-48C0-87DF-BA03AE87A974}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:shape val="box"/>
+        <c:axId val="267324063"/>
+        <c:axId val="267319743"/>
+        <c:axId val="463152175"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="267324063"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Nasa Actual</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>   vs   Simulation</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1280,7 +2041,541 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="286">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1831,6 +3126,110 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59C129F4-DCC7-DEBA-39E6-0450757567AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="438150" y="12325350"/>
+          <a:ext cx="11877675" cy="1400175"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>150203</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>222005</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>424962</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>161192</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D28A2DD2-5ABD-4C7E-9D48-42F8D6F751EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3672ADC9-EF68-4F40-B92B-2DA91F55B736}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2175,8 +3574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87ECA6CB-7DE9-4962-BB31-2ECBD6500398}">
   <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2190,21 +3589,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="28.5" x14ac:dyDescent="0.3">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
     </row>
     <row r="2" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I2" s="2"/>
@@ -2212,202 +3611,202 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:14" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="23" t="s">
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="23" t="s">
+      <c r="G3" s="39"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="23" t="s">
+      <c r="J3" s="39"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="24"/>
-      <c r="N3" s="25"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="40"/>
     </row>
     <row r="4" spans="1:14" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="35" t="s">
+      <c r="B4" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="36" t="s">
+      <c r="D4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="36" t="s">
+      <c r="G4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="35" t="s">
+      <c r="I4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="36" t="s">
+      <c r="J4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="35" t="s">
+      <c r="L4" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="36" t="s">
+      <c r="M4" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="37" t="s">
+      <c r="N4" s="26" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="21.75" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="26">
+      <c r="B5" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="30">
         <v>54.6</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="31">
         <v>46</v>
       </c>
-      <c r="E5" s="28">
+      <c r="E5" s="21">
         <f t="shared" ref="E5" si="0">(C5-D5)/C5</f>
         <v>0.15750915750915753</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="30">
         <v>106.6</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5" s="31">
         <v>107.5</v>
       </c>
-      <c r="H5" s="28">
+      <c r="H5" s="21">
         <f t="shared" ref="H5" si="1">(F5-G5)/F5</f>
         <v>-8.4427767354597165E-3</v>
       </c>
-      <c r="I5" s="26">
+      <c r="I5" s="30">
         <v>148.30000000000001</v>
       </c>
-      <c r="J5" s="27">
+      <c r="J5" s="31">
         <v>147.1</v>
       </c>
-      <c r="K5" s="28">
+      <c r="K5" s="21">
         <f t="shared" ref="K5" si="2">(I5-J5)/I5</f>
         <v>8.0917060013487325E-3</v>
       </c>
-      <c r="L5" s="26">
+      <c r="L5" s="30">
         <v>225.6</v>
       </c>
-      <c r="M5" s="27">
+      <c r="M5" s="31">
         <v>206.7</v>
       </c>
-      <c r="N5" s="28">
+      <c r="N5" s="21">
         <f t="shared" ref="N5" si="3">(L5-M5)/L5</f>
         <v>8.3776595744680882E-2</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="21" x14ac:dyDescent="0.3">
-      <c r="B6" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="29">
+      <c r="B6" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="32">
         <v>56.9</v>
       </c>
-      <c r="D6" s="30">
+      <c r="D6" s="33">
         <v>57.9</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="22">
         <f>(C6-D6)/C6</f>
         <v>-1.7574692442882251E-2</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="32">
         <v>108.1</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="33">
         <v>108.2</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="22">
         <f>(F6-G6)/F6</f>
         <v>-9.2506938020359424E-4</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="32">
         <v>149.4</v>
       </c>
-      <c r="J6" s="30">
+      <c r="J6" s="33">
         <v>149.6</v>
       </c>
-      <c r="K6" s="31">
+      <c r="K6" s="22">
         <f>(I6-J6)/I6</f>
         <v>-1.3386880856759613E-3</v>
       </c>
-      <c r="L6" s="29">
+      <c r="L6" s="32">
         <v>226</v>
       </c>
-      <c r="M6" s="30">
+      <c r="M6" s="33">
         <v>228</v>
       </c>
-      <c r="N6" s="31">
+      <c r="N6" s="22">
         <f>(L6-M6)/L6</f>
         <v>-8.8495575221238937E-3</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="32">
+      <c r="B7" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="34">
         <v>59.1</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="35">
         <v>69.8</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="23">
         <f t="shared" ref="E7" si="4">(C7-D7)/C7</f>
         <v>-0.18104906937394238</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="34">
         <v>109.6</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7" s="35">
         <v>108.9</v>
       </c>
-      <c r="H7" s="34">
+      <c r="H7" s="23">
         <f t="shared" ref="H7" si="5">(F7-G7)/F7</f>
         <v>6.3868613138685099E-3</v>
       </c>
-      <c r="I7" s="32">
+      <c r="I7" s="34">
         <v>150.9</v>
       </c>
-      <c r="J7" s="33">
+      <c r="J7" s="35">
         <v>152.1</v>
       </c>
-      <c r="K7" s="34">
+      <c r="K7" s="23">
         <f t="shared" ref="K7" si="6">(I7-J7)/I7</f>
         <v>-7.9522862823060876E-3</v>
       </c>
-      <c r="L7" s="32">
+      <c r="L7" s="34">
         <v>228.4</v>
       </c>
-      <c r="M7" s="33">
+      <c r="M7" s="35">
         <v>249.3</v>
       </c>
-      <c r="N7" s="34">
+      <c r="N7" s="23">
         <f t="shared" ref="N7" si="7">(L7-M7)/L7</f>
         <v>-9.1506129597197922E-2</v>
       </c>
@@ -2418,39 +3817,39 @@
         <v>16</v>
       </c>
       <c r="C9" s="11">
-        <f>AVERAGE(C6:C7)</f>
-        <v>58</v>
+        <f>AVERAGE(C5:C7)</f>
+        <v>56.866666666666667</v>
       </c>
       <c r="D9" s="11">
-        <f t="shared" ref="D9:M9" si="8">AVERAGE(D6:D7)</f>
-        <v>63.849999999999994</v>
+        <f>AVERAGE(D5:D7)</f>
+        <v>57.9</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11">
-        <f t="shared" si="8"/>
-        <v>108.85</v>
+        <f>AVERAGE(F5:F7)</f>
+        <v>108.09999999999998</v>
       </c>
       <c r="G9" s="11">
-        <f t="shared" si="8"/>
-        <v>108.55000000000001</v>
+        <f>AVERAGE(G5:G7)</f>
+        <v>108.2</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11">
-        <f t="shared" si="8"/>
-        <v>150.15</v>
+        <f>AVERAGE(I5:I7)</f>
+        <v>149.53333333333333</v>
       </c>
       <c r="J9" s="11">
-        <f t="shared" si="8"/>
-        <v>150.85</v>
+        <f>AVERAGE(J5:J7)</f>
+        <v>149.6</v>
       </c>
       <c r="K9" s="11"/>
       <c r="L9" s="11">
-        <f t="shared" si="8"/>
-        <v>227.2</v>
+        <f>AVERAGE(L5:L7)</f>
+        <v>226.66666666666666</v>
       </c>
       <c r="M9" s="11">
-        <f t="shared" si="8"/>
-        <v>238.65</v>
+        <f>AVERAGE(M5:M7)</f>
+        <v>228</v>
       </c>
       <c r="N9" s="11"/>
     </row>
@@ -2564,18 +3963,18 @@
       <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C26" s="19" t="s">
+      <c r="C26" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C27" s="2" t="s">
@@ -2608,51 +4007,51 @@
         <v>13</v>
       </c>
       <c r="C28" s="2">
-        <f t="shared" ref="C28:D30" si="9">C5/$B$11</f>
+        <f t="shared" ref="C28:D30" si="8">C5/$B$11</f>
         <v>0.36497845687585717</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>0.3074910076243485</v>
       </c>
       <c r="E28" s="17">
-        <f t="shared" ref="E28:E30" si="10">(C28-D28)/C28</f>
+        <f t="shared" ref="E28:E30" si="9">(C28-D28)/C28</f>
         <v>0.15750915750915759</v>
       </c>
       <c r="F28" s="2">
-        <f t="shared" ref="F28:G30" si="11">F5/$B$11</f>
+        <f t="shared" ref="F28:G30" si="10">F5/$B$11</f>
         <v>0.71257698723381635</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>0.71859311564385797</v>
       </c>
       <c r="H28" s="17">
-        <f t="shared" ref="H28:H30" si="12">(F28-G28)/F28</f>
+        <f t="shared" ref="H28:H30" si="11">(F28-G28)/F28</f>
         <v>-8.4427767354596905E-3</v>
       </c>
       <c r="I28" s="2">
-        <f t="shared" ref="I28:J30" si="13">I5/$B$11</f>
+        <f t="shared" ref="I28:J30" si="12">I5/$B$11</f>
         <v>0.99132427023241065</v>
       </c>
       <c r="J28" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0.98330276568568842</v>
       </c>
       <c r="K28" s="17">
-        <f t="shared" ref="K28:K30" si="14">(I28-J28)/I28</f>
+        <f t="shared" ref="K28:K30" si="13">(I28-J28)/I28</f>
         <v>8.0917060013487186E-3</v>
       </c>
       <c r="L28" s="2">
-        <f t="shared" ref="L28:M30" si="15">L5/$B$11</f>
+        <f t="shared" ref="L28:M30" si="14">L5/$B$11</f>
         <v>1.5080428547837614</v>
       </c>
       <c r="M28" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.3817041581728877</v>
       </c>
       <c r="N28" s="17">
-        <f t="shared" ref="N28:N30" si="16">(L28-M28)/L28</f>
+        <f t="shared" ref="N28:N30" si="15">(L28-M28)/L28</f>
         <v>8.377659574468091E-2</v>
       </c>
     </row>
@@ -2661,51 +4060,51 @@
         <v>14</v>
       </c>
       <c r="C29" s="2">
+        <f t="shared" si="8"/>
+        <v>0.38035300725707455</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="8"/>
+        <v>0.38703759437934304</v>
+      </c>
+      <c r="E29" s="17">
         <f t="shared" si="9"/>
-        <v>0.38035300725707455</v>
-      </c>
-      <c r="D29" s="2">
-        <f t="shared" si="9"/>
-        <v>0.38703759437934304</v>
-      </c>
-      <c r="E29" s="17">
+        <v>-1.7574692442882373E-2</v>
+      </c>
+      <c r="F29" s="2">
         <f t="shared" si="10"/>
-        <v>-1.7574692442882373E-2</v>
-      </c>
-      <c r="F29" s="2">
+        <v>0.72260386791721898</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="10"/>
+        <v>0.72327232662944585</v>
+      </c>
+      <c r="H29" s="17">
         <f t="shared" si="11"/>
-        <v>0.72260386791721898</v>
-      </c>
-      <c r="G29" s="2">
-        <f t="shared" si="11"/>
-        <v>0.72327232662944585</v>
-      </c>
-      <c r="H29" s="17">
+        <v>-9.250693802035525E-4</v>
+      </c>
+      <c r="I29" s="2">
         <f t="shared" si="12"/>
-        <v>-9.250693802035525E-4</v>
-      </c>
-      <c r="I29" s="2">
+        <v>0.99867731606690591</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="12"/>
+        <v>1.0000142334913595</v>
+      </c>
+      <c r="K29" s="17">
         <f t="shared" si="13"/>
-        <v>0.99867731606690591</v>
-      </c>
-      <c r="J29" s="2">
-        <f t="shared" si="13"/>
-        <v>1.0000142334913595</v>
-      </c>
-      <c r="K29" s="17">
+        <v>-1.33868808567598E-3</v>
+      </c>
+      <c r="L29" s="2">
         <f t="shared" si="14"/>
-        <v>-1.33868808567598E-3</v>
-      </c>
-      <c r="L29" s="2">
+        <v>1.5107166896326689</v>
+      </c>
+      <c r="M29" s="2">
+        <f t="shared" si="14"/>
+        <v>1.5240858638772057</v>
+      </c>
+      <c r="N29" s="17">
         <f t="shared" si="15"/>
-        <v>1.5107166896326689</v>
-      </c>
-      <c r="M29" s="2">
-        <f t="shared" si="15"/>
-        <v>1.5240858638772057</v>
-      </c>
-      <c r="N29" s="17">
-        <f t="shared" si="16"/>
         <v>-8.8495575221238087E-3</v>
       </c>
     </row>
@@ -2714,51 +4113,51 @@
         <v>15</v>
       </c>
       <c r="C30" s="2">
+        <f t="shared" si="8"/>
+        <v>0.39505909892606517</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="8"/>
+        <v>0.46658418113433753</v>
+      </c>
+      <c r="E30" s="17">
         <f t="shared" si="9"/>
-        <v>0.39505909892606517</v>
-      </c>
-      <c r="D30" s="2">
-        <f t="shared" si="9"/>
-        <v>0.46658418113433753</v>
-      </c>
-      <c r="E30" s="17">
+        <v>-0.18104906937394244</v>
+      </c>
+      <c r="F30" s="2">
         <f t="shared" si="10"/>
-        <v>-0.18104906937394244</v>
-      </c>
-      <c r="F30" s="2">
+        <v>0.73263074860062161</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="10"/>
+        <v>0.72795153761503384</v>
+      </c>
+      <c r="H30" s="17">
         <f t="shared" si="11"/>
-        <v>0.73263074860062161</v>
-      </c>
-      <c r="G30" s="2">
-        <f t="shared" si="11"/>
-        <v>0.72795153761503384</v>
-      </c>
-      <c r="H30" s="17">
+        <v>6.3868613138684163E-3</v>
+      </c>
+      <c r="I30" s="2">
         <f t="shared" si="12"/>
-        <v>6.3868613138684163E-3</v>
-      </c>
-      <c r="I30" s="2">
+        <v>1.0087041967503085</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="12"/>
+        <v>1.0167257012970305</v>
+      </c>
+      <c r="K30" s="17">
         <f t="shared" si="13"/>
-        <v>1.0087041967503085</v>
-      </c>
-      <c r="J30" s="2">
-        <f t="shared" si="13"/>
-        <v>1.0167257012970305</v>
-      </c>
-      <c r="K30" s="17">
+        <v>-7.9522862823060425E-3</v>
+      </c>
+      <c r="L30" s="2">
         <f t="shared" si="14"/>
-        <v>-7.9522862823060425E-3</v>
-      </c>
-      <c r="L30" s="2">
+        <v>1.5267596987261132</v>
+      </c>
+      <c r="M30" s="2">
+        <f t="shared" si="14"/>
+        <v>1.6664675695815236</v>
+      </c>
+      <c r="N30" s="17">
         <f t="shared" si="15"/>
-        <v>1.5267596987261132</v>
-      </c>
-      <c r="M30" s="2">
-        <f t="shared" si="15"/>
-        <v>1.6664675695815236</v>
-      </c>
-      <c r="N30" s="17">
-        <f t="shared" si="16"/>
         <v>-9.1506129597197866E-2</v>
       </c>
     </row>
@@ -2793,7 +4192,7 @@
         <v>46</v>
       </c>
       <c r="E38" s="10">
-        <f t="shared" ref="E38" si="17">(C38-D38)/C38</f>
+        <f t="shared" ref="E38" si="16">(C38-D38)/C38</f>
         <v>0.15750915750915753</v>
       </c>
       <c r="F38" s="8">
@@ -2803,7 +4202,7 @@
         <v>107.5</v>
       </c>
       <c r="H38" s="10">
-        <f t="shared" ref="H38" si="18">(F38-G38)/F38</f>
+        <f t="shared" ref="H38" si="17">(F38-G38)/F38</f>
         <v>-8.4427767354597165E-3</v>
       </c>
       <c r="I38" s="8">
@@ -2813,7 +4212,7 @@
         <v>147.1</v>
       </c>
       <c r="K38" s="10">
-        <f t="shared" ref="K38" si="19">(I38-J38)/I38</f>
+        <f t="shared" ref="K38" si="18">(I38-J38)/I38</f>
         <v>8.0917060013487325E-3</v>
       </c>
       <c r="L38" s="8">
@@ -2823,7 +4222,7 @@
         <v>206.7</v>
       </c>
       <c r="N38" s="10">
-        <f t="shared" ref="N38" si="20">(L38-M38)/L38</f>
+        <f t="shared" ref="N38" si="19">(L38-M38)/L38</f>
         <v>8.3776595744680882E-2</v>
       </c>
     </row>
@@ -2873,39 +4272,39 @@
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C59" s="40" t="s">
+      <c r="C59" s="28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C60" s="28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C61" s="28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C60" s="40" t="s">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C62" s="28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C61" s="40" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C62" s="40" t="s">
-        <v>28</v>
-      </c>
-    </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C63" s="40"/>
+      <c r="C63" s="28"/>
     </row>
     <row r="64" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C64" s="40"/>
+      <c r="C64" s="28"/>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C65" s="40"/>
+      <c r="C65" s="28"/>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C66" s="40"/>
+      <c r="C66" s="28"/>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C67" s="40"/>
+      <c r="C67" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2923,4 +4322,758 @@
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
   <drawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ED98602-EC3F-426E-B190-DE720C266919}">
+  <dimension ref="A1:N67"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.59765625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="1" customWidth="1"/>
+    <col min="3" max="5" width="8.796875" style="2" customWidth="1"/>
+    <col min="6" max="14" width="8.796875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="4.59765625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="28.5" x14ac:dyDescent="0.3">
+      <c r="B1" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+    </row>
+    <row r="2" spans="1:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" ht="22.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="39"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="39"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="M3" s="39"/>
+      <c r="N3" s="40"/>
+    </row>
+    <row r="4" spans="1:14" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="21.75" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="30">
+        <v>54.6</v>
+      </c>
+      <c r="D5" s="31">
+        <v>46</v>
+      </c>
+      <c r="E5" s="21">
+        <f t="shared" ref="E5" si="0">(C5-D5)/C5</f>
+        <v>0.15750915750915753</v>
+      </c>
+      <c r="F5" s="30">
+        <v>106.6</v>
+      </c>
+      <c r="G5" s="31">
+        <v>107.5</v>
+      </c>
+      <c r="H5" s="21">
+        <f t="shared" ref="H5" si="1">(F5-G5)/F5</f>
+        <v>-8.4427767354597165E-3</v>
+      </c>
+      <c r="I5" s="30">
+        <v>148.30000000000001</v>
+      </c>
+      <c r="J5" s="31">
+        <v>147.1</v>
+      </c>
+      <c r="K5" s="21">
+        <f t="shared" ref="K5" si="2">(I5-J5)/I5</f>
+        <v>8.0917060013487325E-3</v>
+      </c>
+      <c r="L5" s="30">
+        <v>225.6</v>
+      </c>
+      <c r="M5" s="31">
+        <v>206.7</v>
+      </c>
+      <c r="N5" s="21">
+        <f t="shared" ref="N5" si="3">(L5-M5)/L5</f>
+        <v>8.3776595744680882E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="21" x14ac:dyDescent="0.3">
+      <c r="B6" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="32">
+        <v>56.9</v>
+      </c>
+      <c r="D6" s="33">
+        <v>57.9</v>
+      </c>
+      <c r="E6" s="22">
+        <f>(C6-D6)/C6</f>
+        <v>-1.7574692442882251E-2</v>
+      </c>
+      <c r="F6" s="32">
+        <v>108.1</v>
+      </c>
+      <c r="G6" s="33">
+        <v>108.2</v>
+      </c>
+      <c r="H6" s="22">
+        <f>(F6-G6)/F6</f>
+        <v>-9.2506938020359424E-4</v>
+      </c>
+      <c r="I6" s="32">
+        <v>149.4</v>
+      </c>
+      <c r="J6" s="33">
+        <v>149.6</v>
+      </c>
+      <c r="K6" s="22">
+        <f>(I6-J6)/I6</f>
+        <v>-1.3386880856759613E-3</v>
+      </c>
+      <c r="L6" s="32">
+        <v>226</v>
+      </c>
+      <c r="M6" s="33">
+        <v>228</v>
+      </c>
+      <c r="N6" s="22">
+        <f>(L6-M6)/L6</f>
+        <v>-8.8495575221238937E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="34">
+        <v>59.1</v>
+      </c>
+      <c r="D7" s="35">
+        <v>69.8</v>
+      </c>
+      <c r="E7" s="23">
+        <f t="shared" ref="E7" si="4">(C7-D7)/C7</f>
+        <v>-0.18104906937394238</v>
+      </c>
+      <c r="F7" s="34">
+        <v>109.6</v>
+      </c>
+      <c r="G7" s="35">
+        <v>108.9</v>
+      </c>
+      <c r="H7" s="23">
+        <f t="shared" ref="H7" si="5">(F7-G7)/F7</f>
+        <v>6.3868613138685099E-3</v>
+      </c>
+      <c r="I7" s="34">
+        <v>150.9</v>
+      </c>
+      <c r="J7" s="35">
+        <v>152.1</v>
+      </c>
+      <c r="K7" s="23">
+        <f t="shared" ref="K7" si="6">(I7-J7)/I7</f>
+        <v>-7.9522862823060876E-3</v>
+      </c>
+      <c r="L7" s="34">
+        <v>228.4</v>
+      </c>
+      <c r="M7" s="35">
+        <v>249.3</v>
+      </c>
+      <c r="N7" s="23">
+        <f t="shared" ref="N7" si="7">(L7-M7)/L7</f>
+        <v>-9.1506129597197922E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="19.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="11">
+        <f>AVERAGE(C5:C7)</f>
+        <v>56.866666666666667</v>
+      </c>
+      <c r="D9" s="11">
+        <f>AVERAGE(D5:D7)</f>
+        <v>57.9</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11">
+        <f>AVERAGE(F5:F7)</f>
+        <v>108.09999999999998</v>
+      </c>
+      <c r="G9" s="11">
+        <f>AVERAGE(G5:G7)</f>
+        <v>108.2</v>
+      </c>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11">
+        <f>AVERAGE(I5:I7)</f>
+        <v>149.53333333333333</v>
+      </c>
+      <c r="J9" s="11">
+        <f>AVERAGE(J5:J7)</f>
+        <v>149.6</v>
+      </c>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11">
+        <f>AVERAGE(L5:L7)</f>
+        <v>226.66666666666666</v>
+      </c>
+      <c r="M9" s="11">
+        <f>AVERAGE(M5:M7)</f>
+        <v>228</v>
+      </c>
+      <c r="N9" s="11"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="16">
+        <v>149.59787069999999</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="F12" s="12"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="15"/>
+      <c r="B13" s="16"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="15"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="15"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="F15" s="12"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="15"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="15"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="F18" s="12"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="F20" s="12"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="15"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="F21" s="12"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="15"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="F22" s="12"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="15"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="15"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="F24" s="12"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A25" s="15"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="F25" s="12"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C26" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B28" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" ref="C28:D30" si="8">C5/$B$11</f>
+        <v>0.36497845687585717</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="8"/>
+        <v>0.3074910076243485</v>
+      </c>
+      <c r="E28" s="17">
+        <f t="shared" ref="E28:E30" si="9">(C28-D28)/C28</f>
+        <v>0.15750915750915759</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" ref="F28:G30" si="10">F5/$B$11</f>
+        <v>0.71257698723381635</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="10"/>
+        <v>0.71859311564385797</v>
+      </c>
+      <c r="H28" s="17">
+        <f t="shared" ref="H28:H30" si="11">(F28-G28)/F28</f>
+        <v>-8.4427767354596905E-3</v>
+      </c>
+      <c r="I28" s="2">
+        <f t="shared" ref="I28:J30" si="12">I5/$B$11</f>
+        <v>0.99132427023241065</v>
+      </c>
+      <c r="J28" s="2">
+        <f t="shared" si="12"/>
+        <v>0.98330276568568842</v>
+      </c>
+      <c r="K28" s="17">
+        <f t="shared" ref="K28:K30" si="13">(I28-J28)/I28</f>
+        <v>8.0917060013487186E-3</v>
+      </c>
+      <c r="L28" s="2">
+        <f t="shared" ref="L28:M30" si="14">L5/$B$11</f>
+        <v>1.5080428547837614</v>
+      </c>
+      <c r="M28" s="2">
+        <f t="shared" si="14"/>
+        <v>1.3817041581728877</v>
+      </c>
+      <c r="N28" s="17">
+        <f t="shared" ref="N28:N30" si="15">(L28-M28)/L28</f>
+        <v>8.377659574468091E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B29" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="8"/>
+        <v>0.38035300725707455</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="8"/>
+        <v>0.38703759437934304</v>
+      </c>
+      <c r="E29" s="17">
+        <f t="shared" si="9"/>
+        <v>-1.7574692442882373E-2</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="10"/>
+        <v>0.72260386791721898</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="10"/>
+        <v>0.72327232662944585</v>
+      </c>
+      <c r="H29" s="17">
+        <f t="shared" si="11"/>
+        <v>-9.250693802035525E-4</v>
+      </c>
+      <c r="I29" s="2">
+        <f t="shared" si="12"/>
+        <v>0.99867731606690591</v>
+      </c>
+      <c r="J29" s="2">
+        <f t="shared" si="12"/>
+        <v>1.0000142334913595</v>
+      </c>
+      <c r="K29" s="17">
+        <f t="shared" si="13"/>
+        <v>-1.33868808567598E-3</v>
+      </c>
+      <c r="L29" s="2">
+        <f t="shared" si="14"/>
+        <v>1.5107166896326689</v>
+      </c>
+      <c r="M29" s="2">
+        <f t="shared" si="14"/>
+        <v>1.5240858638772057</v>
+      </c>
+      <c r="N29" s="17">
+        <f t="shared" si="15"/>
+        <v>-8.8495575221238087E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B30" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="8"/>
+        <v>0.39505909892606517</v>
+      </c>
+      <c r="D30" s="2">
+        <f t="shared" si="8"/>
+        <v>0.46658418113433753</v>
+      </c>
+      <c r="E30" s="17">
+        <f t="shared" si="9"/>
+        <v>-0.18104906937394244</v>
+      </c>
+      <c r="F30" s="2">
+        <f t="shared" si="10"/>
+        <v>0.73263074860062161</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="10"/>
+        <v>0.72795153761503384</v>
+      </c>
+      <c r="H30" s="17">
+        <f t="shared" si="11"/>
+        <v>6.3868613138684163E-3</v>
+      </c>
+      <c r="I30" s="2">
+        <f t="shared" si="12"/>
+        <v>1.0087041967503085</v>
+      </c>
+      <c r="J30" s="2">
+        <f t="shared" si="12"/>
+        <v>1.0167257012970305</v>
+      </c>
+      <c r="K30" s="17">
+        <f t="shared" si="13"/>
+        <v>-7.9522862823060425E-3</v>
+      </c>
+      <c r="L30" s="2">
+        <f t="shared" si="14"/>
+        <v>1.5267596987261132</v>
+      </c>
+      <c r="M30" s="2">
+        <f t="shared" si="14"/>
+        <v>1.6664675695815236</v>
+      </c>
+      <c r="N30" s="17">
+        <f t="shared" si="15"/>
+        <v>-9.1506129597197866E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="D32" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="I33" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="I34" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="I35" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" ht="21.75" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="8">
+        <v>54.6</v>
+      </c>
+      <c r="D38" s="9">
+        <v>46</v>
+      </c>
+      <c r="E38" s="10">
+        <f t="shared" ref="E38" si="16">(C38-D38)/C38</f>
+        <v>0.15750915750915753</v>
+      </c>
+      <c r="F38" s="8">
+        <v>106.6</v>
+      </c>
+      <c r="G38" s="9">
+        <v>107.5</v>
+      </c>
+      <c r="H38" s="10">
+        <f t="shared" ref="H38" si="17">(F38-G38)/F38</f>
+        <v>-8.4427767354597165E-3</v>
+      </c>
+      <c r="I38" s="8">
+        <v>148.30000000000001</v>
+      </c>
+      <c r="J38" s="9">
+        <v>147.1</v>
+      </c>
+      <c r="K38" s="10">
+        <f t="shared" ref="K38" si="18">(I38-J38)/I38</f>
+        <v>8.0917060013487325E-3</v>
+      </c>
+      <c r="L38" s="8">
+        <v>225.6</v>
+      </c>
+      <c r="M38" s="9">
+        <v>206.7</v>
+      </c>
+      <c r="N38" s="10">
+        <f t="shared" ref="N38" si="19">(L38-M38)/L38</f>
+        <v>8.3776595744680882E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" ht="21.75" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="5">
+        <v>56.9</v>
+      </c>
+      <c r="D39" s="6">
+        <v>57.9</v>
+      </c>
+      <c r="E39" s="7">
+        <f>(C39-D39)/C39</f>
+        <v>-1.7574692442882251E-2</v>
+      </c>
+      <c r="F39" s="5">
+        <v>108.1</v>
+      </c>
+      <c r="G39" s="6">
+        <v>108.2</v>
+      </c>
+      <c r="H39" s="7">
+        <f>(F39-G39)/F39</f>
+        <v>-9.2506938020359424E-4</v>
+      </c>
+      <c r="I39" s="5">
+        <v>149.4</v>
+      </c>
+      <c r="J39" s="6">
+        <v>149.6</v>
+      </c>
+      <c r="K39" s="7">
+        <f>(I39-J39)/I39</f>
+        <v>-1.3386880856759613E-3</v>
+      </c>
+      <c r="L39" s="5">
+        <v>226</v>
+      </c>
+      <c r="M39" s="6">
+        <v>228</v>
+      </c>
+      <c r="N39" s="7">
+        <f>(L39-M39)/L39</f>
+        <v>-8.8495575221238937E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C59" s="28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C60" s="28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C61" s="28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C62" s="28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C63" s="28"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C64" s="28"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C65" s="28"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C66" s="28"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C67" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:N1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="C26:L26"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D32" r:id="rId1" xr:uid="{2217FCF0-C4BC-47B6-B7D9-A355AE8A9E07}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>